<commit_message>
updates to network creation (allow for parameterisation to account for genuine islands like Hong Kong), and public open space identification (boundary=protected_area is no longer used to identify open space; instead it is assumed that most cases with this tag which are considered to be in the spirit of public open space will have an additional 'leisure' tag, or otherwise be indicated to be like a national park etc; this will reduce potential large scale false/problematic positives like UNESCO world heritage areas -ie. Graz old centre- which if identified as public open space are not sampled within.  So this commit addresses those issues.
</commit_message>
<xml_diff>
--- a/process/pre_process/_project_configuration.xlsx
+++ b/process/pre_process/_project_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\global-indicators\process\pre_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E732D51-13A6-4EDF-9196-1A8BA3CFB328}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB30C07A-A92A-487F-8F65-DDCB3BF7F1B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="16" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="618">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="627">
   <si>
     <t>notes</t>
   </si>
@@ -1998,6 +1998,33 @@
   </si>
   <si>
     <t>If false, only retain main connected network when retrieving OSM roads</t>
+  </si>
+  <si>
+    <t>network</t>
+  </si>
+  <si>
+    <t>Second pass criteria (removed boundary=protected_area)</t>
+  </si>
+  <si>
+    <t>national_park,nature_reserve,forest,state_forest,state_park,regional_park,park,county_park</t>
+  </si>
+  <si>
+    <t>network_not_using_buffered_region</t>
+  </si>
+  <si>
+    <t>Instead of using buffered study region, use regular study region for excerpting network from OSM.  This may allow for looping over true islands to extract individual networks (eg. Hong Kong), which may not be possible with the buffered region (which results in only retaining larget network segment)</t>
+  </si>
+  <si>
+    <t>network_connection_threshold</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Minimum distance to retain </t>
+  </si>
+  <si>
+    <t>network_polygon_iteration</t>
+  </si>
+  <si>
+    <t>Iterate over polygons for network retrieval, and then combin</t>
   </si>
 </sst>
 </file>
@@ -3471,8 +3498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF89BF1A-C929-463D-A334-3406512FE43F}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4025,10 +4052,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737B355D-4426-4406-A37B-14B20C191AA3}">
-  <dimension ref="A1:AB14"/>
+  <dimension ref="A1:AB17"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:AB1"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4906,6 +4933,48 @@
       </c>
       <c r="V14" t="s">
         <v>468</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>621</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>622</v>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>625</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>623</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>618</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="J17">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -6385,7 +6454,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B72" sqref="B72"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6577,7 +6646,7 @@
   </sheetPr>
   <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
@@ -7876,10 +7945,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6A12AB-4082-428A-9AD8-30AFCF82C953}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7887,12 +7956,12 @@
     <col min="1" max="1" width="22.140625" style="3" customWidth="1"/>
     <col min="2" max="4" width="32.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="84" style="5" customWidth="1"/>
-    <col min="6" max="6" width="49.85546875" style="5" customWidth="1"/>
-    <col min="7" max="7" width="55.28515625" style="56" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="3"/>
+    <col min="6" max="7" width="49.85546875" style="5" customWidth="1"/>
+    <col min="8" max="8" width="55.28515625" style="56" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>494</v>
       </c>
@@ -7911,11 +7980,14 @@
       <c r="F1" s="10" t="s">
         <v>495</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="10" t="s">
+        <v>619</v>
+      </c>
+      <c r="H1" s="58" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>493</v>
       </c>
@@ -7929,10 +8001,13 @@
         <v>574</v>
       </c>
       <c r="G2" s="57" t="s">
+        <v>574</v>
+      </c>
+      <c r="H2" s="57" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>492</v>
       </c>
@@ -7952,10 +8027,13 @@
         <v>576</v>
       </c>
       <c r="G3" s="57" t="s">
+        <v>576</v>
+      </c>
+      <c r="H3" s="57" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>127</v>
       </c>
@@ -7975,10 +8053,13 @@
         <v>579</v>
       </c>
       <c r="G4" s="57" t="s">
+        <v>579</v>
+      </c>
+      <c r="H4" s="57" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>129</v>
       </c>
@@ -7995,13 +8076,16 @@
         <v>502</v>
       </c>
       <c r="F5" s="5" t="s">
+        <v>620</v>
+      </c>
+      <c r="G5" s="57" t="s">
         <v>566</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="H5" s="57" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>489</v>
       </c>
@@ -8023,8 +8107,11 @@
       <c r="G6" s="57" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H6" s="57" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>490</v>
       </c>
@@ -8046,8 +8133,11 @@
       <c r="G7" s="57" t="s">
         <v>514</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="H7" s="57" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>571</v>
       </c>
@@ -8067,10 +8157,13 @@
         <v>569</v>
       </c>
       <c r="G8" s="57" t="s">
+        <v>569</v>
+      </c>
+      <c r="H8" s="57" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>491</v>
       </c>
@@ -8092,8 +8185,11 @@
       <c r="G9" s="57" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H9" s="57" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>564</v>
       </c>
@@ -8115,8 +8211,11 @@
       <c r="G10" s="57" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="H10" s="57" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>147</v>
       </c>
@@ -8132,8 +8231,11 @@
       <c r="G11" s="57" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H11" s="57" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>149</v>
       </c>
@@ -8155,8 +8257,11 @@
       <c r="G12" s="57" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="H12" s="57" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>151</v>
       </c>
@@ -8176,8 +8281,11 @@
       <c r="G13" s="57" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="H13" s="57" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>155</v>
       </c>
@@ -8197,10 +8305,13 @@
         <v>580</v>
       </c>
       <c r="G14" s="57" t="s">
+        <v>580</v>
+      </c>
+      <c r="H14" s="57" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>157</v>
       </c>
@@ -8220,6 +8331,9 @@
         <v>568</v>
       </c>
       <c r="G15" s="57" t="s">
+        <v>568</v>
+      </c>
+      <c r="H15" s="57" t="s">
         <v>214</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated destination compilation code and setup files to allow for ingestion of custom destination data
</commit_message>
<xml_diff>
--- a/process/pre_process/_project_configuration.xlsx
+++ b/process/pre_process/_project_configuration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\global-indicators\process\pre_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB30C07A-A92A-487F-8F65-DDCB3BF7F1B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF9CFF5-4617-4FA2-ABBC-A9B962DCD1FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1282" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="630">
   <si>
     <t>notes</t>
   </si>
@@ -2025,6 +2025,15 @@
   </si>
   <si>
     <t>Iterate over polygons for network retrieval, and then combin</t>
+  </si>
+  <si>
+    <t>custom_destinations</t>
+  </si>
+  <si>
+    <t>Custom destinations to use, in addition to those from OSM.  Use a comma seperated list specifying file name (located in study region folder, once generated), category plain name field, category full name field, Y coordinate, X coordinate, EPSG number</t>
+  </si>
+  <si>
+    <t>Maiduguri_shops_convenience_complete_2020-07-13_categorised_final.csv,dest_name,dest_name_full,Latitude,Longitude,4326</t>
   </si>
 </sst>
 </file>
@@ -4052,10 +4061,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737B355D-4426-4406-A37B-14B20C191AA3}">
-  <dimension ref="A1:AB17"/>
+  <dimension ref="A1:AB18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4975,6 +4984,20 @@
       </c>
       <c r="J17">
         <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>627</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>628</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated docker image and code associated with validation report  --- now accounts for custom destinations where provided, including custom destination attribution.  In addition, all cities report tables are now generated in latex from Pandas, instead of compiled manually from CSVs (looks almost as good, but took a lot of coding to get it that way - but is now generalisable and run on demand which is ideal)
</commit_message>
<xml_diff>
--- a/process/pre_process/_project_configuration.xlsx
+++ b/process/pre_process/_project_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\global-indicators\process\pre_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF9CFF5-4617-4FA2-ABBC-A9B962DCD1FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0ACAD3E-4D96-4C1F-B50C-D9B5B8A312D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="16" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">datasets!$A$1:$AP$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">destinations!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">project_settings!$A$1:$D$35</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2">region_settings!$A$1:$X$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2">region_settings!$A$1:$X$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="662">
   <si>
     <t>notes</t>
   </si>
@@ -967,9 +967,6 @@
     <t>Full study region name</t>
   </si>
   <si>
-    <t>Broader region where study region is located</t>
-  </si>
-  <si>
     <t>Downloaded OpenStreetMap (OSM) data</t>
   </si>
   <si>
@@ -2034,6 +2031,105 @@
   </si>
   <si>
     <t>Maiduguri_shops_convenience_complete_2020-07-13_categorised_final.csv,dest_name,dest_name_full,Latitude,Longitude,4326</t>
+  </si>
+  <si>
+    <t>continent</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Fully country name</t>
+  </si>
+  <si>
+    <t>Continent name</t>
+  </si>
+  <si>
+    <t>Nigeria</t>
+  </si>
+  <si>
+    <t>Two character country code (ISO3166 Alpha-2 code)</t>
+  </si>
+  <si>
+    <t>Africa</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>America, North</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>America, South</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Thailand</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>Austria</t>
+  </si>
+  <si>
+    <t>Europe</t>
+  </si>
+  <si>
+    <t>Belgium</t>
+  </si>
+  <si>
+    <t>Switzerland</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Czech Republic </t>
+  </si>
+  <si>
+    <t>Germany</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>Portugal</t>
+  </si>
+  <si>
+    <t>Australia</t>
+  </si>
+  <si>
+    <t>Australasia</t>
+  </si>
+  <si>
+    <t>New Zealand</t>
+  </si>
+  <si>
+    <t>China (SAR)</t>
+  </si>
+  <si>
+    <t>United Kingdom</t>
+  </si>
+  <si>
+    <t>custom_destinations_attribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom destination attribution </t>
+  </si>
+  <si>
+    <t>Dr Garba Sambo (University of Maiduguri) and Assoc. Prof. Adewale Oyeyemi (University of Maiduguri)</t>
   </si>
 </sst>
 </file>
@@ -2727,8 +2823,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2740,7 +2836,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -2751,7 +2847,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2771,7 +2867,7 @@
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2884,18 +2980,18 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B21" s="20"/>
       <c r="C21" s="52" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="7"/>
       <c r="C22" s="5" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D22" s="21"/>
     </row>
@@ -2909,11 +3005,11 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B24" s="26"/>
       <c r="C24" s="4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>91</v>
@@ -3544,7 +3640,7 @@
         <v>35</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3591,16 +3687,16 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3653,7 +3749,7 @@
         <v>34</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D10" s="14">
         <v>0</v>
@@ -3667,7 +3763,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D11" s="14">
         <v>2020</v>
@@ -3675,7 +3771,7 @@
     </row>
     <row r="12" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>54</v>
@@ -3748,24 +3844,24 @@
         <v>204</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>282</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>294</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>283</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>295</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>284</v>
       </c>
       <c r="D18" s="14">
         <v>20200813</v>
@@ -3773,13 +3869,13 @@
     </row>
     <row r="19" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>293</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>295</v>
-      </c>
       <c r="C19" s="2" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D19" s="14" t="str">
         <f>"False"</f>
@@ -3808,21 +3904,21 @@
         <v>61</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>304</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>305</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D22" s="14">
         <v>30</v>
@@ -3956,41 +4052,41 @@
     </row>
     <row r="32" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>297</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="14" t="s">
         <v>300</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="33" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>322</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>324</v>
-      </c>
       <c r="C33" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D33" s="14" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="34" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>324</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>325</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>326</v>
       </c>
       <c r="D34" s="14">
         <v>1.1000000000000001</v>
@@ -3998,41 +4094,41 @@
     </row>
     <row r="35" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>327</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>324</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>329</v>
-      </c>
       <c r="D35" s="14" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="D36" s="14" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>435</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>436</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>437</v>
-      </c>
       <c r="C37" s="2" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D37" s="14">
         <v>2015</v>
@@ -4040,16 +4136,16 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>446</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>448</v>
-      </c>
       <c r="C38" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
   </sheetData>
@@ -4061,10 +4157,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737B355D-4426-4406-A37B-14B20C191AA3}">
-  <dimension ref="A1:AB18"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4089,79 +4185,79 @@
         <v>32</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E1" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>403</v>
       </c>
-      <c r="F1" s="16" t="s">
-        <v>404</v>
-      </c>
       <c r="G1" s="16" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>272</v>
       </c>
       <c r="M1" s="16" t="s">
+        <v>373</v>
+      </c>
+      <c r="N1" s="16" t="s">
+        <v>404</v>
+      </c>
+      <c r="O1" s="16" t="s">
         <v>374</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="P1" s="16" t="s">
         <v>405</v>
       </c>
-      <c r="O1" s="16" t="s">
+      <c r="Q1" s="16" t="s">
+        <v>376</v>
+      </c>
+      <c r="R1" s="16" t="s">
+        <v>406</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>377</v>
+      </c>
+      <c r="T1" s="16" t="s">
+        <v>371</v>
+      </c>
+      <c r="U1" s="16" t="s">
+        <v>379</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>370</v>
+      </c>
+      <c r="X1" s="16" t="s">
+        <v>407</v>
+      </c>
+      <c r="Y1" s="16" t="s">
+        <v>369</v>
+      </c>
+      <c r="Z1" s="16" t="s">
         <v>375</v>
       </c>
-      <c r="P1" s="16" t="s">
-        <v>406</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>377</v>
-      </c>
-      <c r="R1" s="16" t="s">
-        <v>407</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>378</v>
-      </c>
-      <c r="T1" s="16" t="s">
-        <v>372</v>
-      </c>
-      <c r="U1" s="16" t="s">
+      <c r="AA1" s="16" t="s">
         <v>380</v>
       </c>
-      <c r="V1" s="16" t="s">
-        <v>379</v>
-      </c>
-      <c r="W1" s="16" t="s">
-        <v>371</v>
-      </c>
-      <c r="X1" s="16" t="s">
-        <v>408</v>
-      </c>
-      <c r="Y1" s="16" t="s">
-        <v>370</v>
-      </c>
-      <c r="Z1" s="16" t="s">
-        <v>376</v>
-      </c>
-      <c r="AA1" s="16" t="s">
-        <v>381</v>
-      </c>
       <c r="AB1" s="16" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.25">
@@ -4261,79 +4357,79 @@
         <v>280</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E3" t="s">
+        <v>408</v>
+      </c>
+      <c r="F3" t="s">
         <v>409</v>
       </c>
-      <c r="F3" t="s">
-        <v>410</v>
-      </c>
       <c r="G3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="J3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="L3" t="s">
         <v>271</v>
       </c>
       <c r="M3" t="s">
+        <v>345</v>
+      </c>
+      <c r="N3" t="s">
+        <v>410</v>
+      </c>
+      <c r="O3" t="s">
         <v>346</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>411</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
+        <v>349</v>
+      </c>
+      <c r="R3" t="s">
+        <v>412</v>
+      </c>
+      <c r="S3" t="s">
+        <v>350</v>
+      </c>
+      <c r="T3" t="s">
+        <v>343</v>
+      </c>
+      <c r="U3" t="s">
+        <v>352</v>
+      </c>
+      <c r="V3" t="s">
+        <v>351</v>
+      </c>
+      <c r="W3" t="s">
+        <v>342</v>
+      </c>
+      <c r="X3" t="s">
+        <v>399</v>
+      </c>
+      <c r="Y3" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="Z3" t="s">
         <v>347</v>
       </c>
-      <c r="P3" t="s">
-        <v>412</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>350</v>
-      </c>
-      <c r="R3" t="s">
-        <v>413</v>
-      </c>
-      <c r="S3" t="s">
-        <v>351</v>
-      </c>
-      <c r="T3" t="s">
-        <v>344</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="AA3" t="s">
         <v>353</v>
       </c>
-      <c r="V3" t="s">
-        <v>352</v>
-      </c>
-      <c r="W3" t="s">
-        <v>343</v>
-      </c>
-      <c r="X3" t="s">
-        <v>400</v>
-      </c>
-      <c r="Y3" s="14" t="s">
-        <v>342</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>348</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>354</v>
-      </c>
       <c r="AB3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -4430,399 +4526,499 @@
         <v>277</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>281</v>
+        <v>634</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="E5" t="s">
         <v>414</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>355</v>
+      </c>
+      <c r="G5" t="s">
+        <v>355</v>
+      </c>
+      <c r="H5" t="s">
+        <v>355</v>
+      </c>
+      <c r="I5" t="s">
+        <v>365</v>
+      </c>
+      <c r="J5" t="s">
+        <v>364</v>
+      </c>
+      <c r="K5" t="s">
+        <v>360</v>
+      </c>
+      <c r="L5" t="s">
+        <v>359</v>
+      </c>
+      <c r="M5" t="s">
+        <v>361</v>
+      </c>
+      <c r="N5" t="s">
         <v>415</v>
       </c>
-      <c r="F5" t="s">
+      <c r="O5" t="s">
+        <v>362</v>
+      </c>
+      <c r="P5" t="s">
+        <v>416</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>366</v>
+      </c>
+      <c r="R5" t="s">
+        <v>417</v>
+      </c>
+      <c r="S5" t="s">
+        <v>367</v>
+      </c>
+      <c r="T5" t="s">
+        <v>358</v>
+      </c>
+      <c r="U5" t="s">
+        <v>358</v>
+      </c>
+      <c r="V5" t="s">
+        <v>358</v>
+      </c>
+      <c r="W5" t="s">
+        <v>357</v>
+      </c>
+      <c r="X5" t="s">
+        <v>363</v>
+      </c>
+      <c r="Y5" s="14" t="s">
         <v>356</v>
       </c>
-      <c r="G5" t="s">
+      <c r="Z5" t="s">
         <v>356</v>
       </c>
-      <c r="H5" t="s">
+      <c r="AA5" t="s">
         <v>356</v>
       </c>
-      <c r="I5" t="s">
-        <v>366</v>
-      </c>
-      <c r="J5" t="s">
-        <v>365</v>
-      </c>
-      <c r="K5" t="s">
-        <v>361</v>
-      </c>
-      <c r="L5" t="s">
-        <v>360</v>
-      </c>
-      <c r="M5" t="s">
-        <v>362</v>
-      </c>
-      <c r="N5" t="s">
-        <v>416</v>
-      </c>
-      <c r="O5" t="s">
-        <v>363</v>
-      </c>
-      <c r="P5" t="s">
-        <v>417</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>367</v>
-      </c>
-      <c r="R5" t="s">
-        <v>418</v>
-      </c>
-      <c r="S5" t="s">
-        <v>368</v>
-      </c>
-      <c r="T5" t="s">
-        <v>359</v>
-      </c>
-      <c r="U5" t="s">
-        <v>359</v>
-      </c>
-      <c r="V5" t="s">
-        <v>359</v>
-      </c>
-      <c r="W5" t="s">
-        <v>358</v>
-      </c>
-      <c r="X5" t="s">
-        <v>364</v>
-      </c>
-      <c r="Y5" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>357</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>357</v>
-      </c>
       <c r="AB5" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>391</v>
+        <v>354</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>630</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C6" s="47" t="s">
-        <v>392</v>
+      <c r="C6" s="2" t="s">
+        <v>631</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>385</v>
-      </c>
-      <c r="E6" s="14" t="s">
-        <v>419</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>420</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>393</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>421</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>384</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>388</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>389</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>422</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>390</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>385</v>
-      </c>
-      <c r="P6" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="Q6" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="R6" s="14" t="s">
-        <v>385</v>
-      </c>
-      <c r="S6" s="14" t="s">
-        <v>386</v>
-      </c>
-      <c r="U6" s="14" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>37</v>
+        <v>633</v>
+      </c>
+      <c r="E6" t="s">
+        <v>636</v>
+      </c>
+      <c r="F6" t="s">
+        <v>638</v>
+      </c>
+      <c r="G6" t="s">
+        <v>638</v>
+      </c>
+      <c r="H6" t="s">
+        <v>638</v>
+      </c>
+      <c r="I6" t="s">
+        <v>639</v>
+      </c>
+      <c r="J6" t="s">
+        <v>657</v>
+      </c>
+      <c r="K6" t="s">
+        <v>642</v>
+      </c>
+      <c r="L6" t="s">
+        <v>643</v>
+      </c>
+      <c r="M6" t="s">
+        <v>644</v>
+      </c>
+      <c r="N6" t="s">
+        <v>645</v>
+      </c>
+      <c r="O6" t="s">
+        <v>647</v>
+      </c>
+      <c r="P6" t="s">
+        <v>648</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>649</v>
+      </c>
+      <c r="R6" t="s">
+        <v>650</v>
+      </c>
+      <c r="S6" t="s">
+        <v>651</v>
+      </c>
+      <c r="T6" t="s">
+        <v>652</v>
+      </c>
+      <c r="U6" t="s">
+        <v>652</v>
+      </c>
+      <c r="V6" t="s">
+        <v>652</v>
+      </c>
+      <c r="W6" t="s">
+        <v>658</v>
+      </c>
+      <c r="X6" t="s">
+        <v>653</v>
+      </c>
+      <c r="Y6" s="14" t="s">
+        <v>654</v>
+      </c>
+      <c r="Z6" s="14" t="s">
+        <v>654</v>
+      </c>
+      <c r="AA6" s="14" t="s">
+        <v>654</v>
+      </c>
+      <c r="AB6" s="14" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>629</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>277</v>
       </c>
-      <c r="C7" s="47" t="s">
+      <c r="C7" s="2" t="s">
+        <v>632</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>635</v>
+      </c>
+      <c r="E7" t="s">
+        <v>637</v>
+      </c>
+      <c r="F7" t="s">
+        <v>637</v>
+      </c>
+      <c r="G7" t="s">
+        <v>637</v>
+      </c>
+      <c r="H7" t="s">
+        <v>637</v>
+      </c>
+      <c r="I7" t="s">
+        <v>640</v>
+      </c>
+      <c r="J7" t="s">
+        <v>641</v>
+      </c>
+      <c r="K7" t="s">
+        <v>641</v>
+      </c>
+      <c r="L7" t="s">
+        <v>641</v>
+      </c>
+      <c r="M7" t="s">
+        <v>641</v>
+      </c>
+      <c r="N7" t="s">
+        <v>646</v>
+      </c>
+      <c r="O7" t="s">
+        <v>646</v>
+      </c>
+      <c r="P7" t="s">
+        <v>646</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>646</v>
+      </c>
+      <c r="R7" t="s">
+        <v>646</v>
+      </c>
+      <c r="S7" t="s">
+        <v>646</v>
+      </c>
+      <c r="T7" t="s">
+        <v>646</v>
+      </c>
+      <c r="U7" t="s">
+        <v>646</v>
+      </c>
+      <c r="V7" t="s">
+        <v>646</v>
+      </c>
+      <c r="W7" t="s">
+        <v>646</v>
+      </c>
+      <c r="X7" t="s">
+        <v>646</v>
+      </c>
+      <c r="Y7" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="Z7" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="AA7" s="14" t="s">
+        <v>655</v>
+      </c>
+      <c r="AB7" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>390</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>391</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>418</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>419</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>383</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>387</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>388</v>
+      </c>
+      <c r="L8" s="14" t="s">
+        <v>421</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>389</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="P8" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q8" s="14" t="s">
+        <v>382</v>
+      </c>
+      <c r="R8" s="14" t="s">
+        <v>384</v>
+      </c>
+      <c r="S8" s="14" t="s">
+        <v>385</v>
+      </c>
+      <c r="U8" s="14" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D9" s="14">
         <v>32633</v>
       </c>
-      <c r="E7" s="14">
+      <c r="E9" s="14">
         <v>32614</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F9" s="14">
         <v>32618</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G9" s="14">
         <v>32612</v>
       </c>
-      <c r="H7" s="14">
+      <c r="H9" s="14">
         <v>32610</v>
       </c>
-      <c r="I7" s="14">
+      <c r="I9" s="14">
         <v>32723</v>
       </c>
-      <c r="J7" s="14">
+      <c r="J9" s="14">
         <v>32650</v>
       </c>
-      <c r="K7" s="14">
+      <c r="K9" s="14">
         <v>32644</v>
       </c>
-      <c r="L7" s="14">
+      <c r="L9" s="14">
         <v>32647</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M9" s="14">
         <v>32648</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N9" s="14">
         <v>32633</v>
       </c>
-      <c r="O7" s="14">
+      <c r="O9" s="14">
         <v>32631</v>
       </c>
-      <c r="P7" s="14">
+      <c r="P9" s="14">
         <v>32633</v>
       </c>
-      <c r="Q7" s="14">
+      <c r="Q9" s="14">
         <v>32633</v>
       </c>
-      <c r="R7" s="14">
+      <c r="R9" s="14">
         <v>32631</v>
       </c>
-      <c r="S7" s="14">
+      <c r="S9" s="14">
         <v>32632</v>
       </c>
-      <c r="T7" s="14">
+      <c r="T9" s="14">
         <v>25831</v>
       </c>
-      <c r="U7" s="14">
+      <c r="U9" s="14">
         <v>25830</v>
       </c>
-      <c r="V7" s="14">
+      <c r="V9" s="14">
         <v>25831</v>
       </c>
-      <c r="W7" s="14">
+      <c r="W9" s="14">
         <v>29902</v>
       </c>
-      <c r="X7" s="14">
+      <c r="X9" s="14">
         <v>3763</v>
       </c>
-      <c r="Y7" s="14">
+      <c r="Y9" s="14">
         <v>7845</v>
       </c>
-      <c r="Z7" s="14">
+      <c r="Z9" s="14">
         <v>7845</v>
       </c>
-      <c r="AA7" s="14">
+      <c r="AA9" s="14">
         <v>7845</v>
       </c>
-      <c r="AB7" s="14">
+      <c r="AB9" s="14">
         <v>2193</v>
       </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>523</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>552</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>583</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>527</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>581</v>
-      </c>
-      <c r="G8" s="39" t="s">
-        <v>529</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>582</v>
-      </c>
-      <c r="I8" s="39" t="s">
-        <v>531</v>
-      </c>
-      <c r="J8" s="39" t="s">
-        <v>532</v>
-      </c>
-      <c r="K8" s="39" t="s">
-        <v>533</v>
-      </c>
-      <c r="L8" s="39" t="s">
-        <v>534</v>
-      </c>
-      <c r="M8" s="39" t="s">
-        <v>535</v>
-      </c>
-      <c r="N8" s="39" t="s">
-        <v>536</v>
-      </c>
-      <c r="O8" s="39" t="s">
-        <v>537</v>
-      </c>
-      <c r="P8" s="39" t="s">
-        <v>538</v>
-      </c>
-      <c r="Q8" s="39" t="s">
-        <v>539</v>
-      </c>
-      <c r="R8" s="39" t="s">
-        <v>540</v>
-      </c>
-      <c r="S8" s="39" t="s">
-        <v>541</v>
-      </c>
-      <c r="T8" s="39" t="s">
-        <v>542</v>
-      </c>
-      <c r="U8" s="39" t="s">
-        <v>543</v>
-      </c>
-      <c r="V8" s="39" t="s">
-        <v>544</v>
-      </c>
-      <c r="W8" s="39" t="s">
-        <v>545</v>
-      </c>
-      <c r="X8" s="39" t="s">
-        <v>546</v>
-      </c>
-      <c r="Y8" s="39" t="s">
-        <v>547</v>
-      </c>
-      <c r="Z8" s="39" t="s">
-        <v>548</v>
-      </c>
-      <c r="AA8" s="39" t="s">
-        <v>549</v>
-      </c>
-      <c r="AB8" s="39" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>553</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>557</v>
-      </c>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
-      <c r="T9" s="39"/>
-      <c r="U9" s="39"/>
-      <c r="V9" s="39"/>
-      <c r="W9" s="39"/>
-      <c r="X9" s="39"/>
-      <c r="Y9" s="39"/>
-      <c r="Z9" s="39"/>
-      <c r="AA9" s="39"/>
-      <c r="AB9" s="39"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>554</v>
+        <v>522</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>558</v>
-      </c>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="39"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="39"/>
-      <c r="Q10" s="39"/>
-      <c r="R10" s="39"/>
-      <c r="S10" s="39"/>
-      <c r="T10" s="39"/>
-      <c r="U10" s="39"/>
-      <c r="V10" s="39"/>
-      <c r="W10" s="39"/>
-      <c r="X10" s="39"/>
-      <c r="Y10" s="39"/>
-      <c r="Z10" s="39"/>
-      <c r="AA10" s="39"/>
-      <c r="AB10" s="39"/>
+        <v>551</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>582</v>
+      </c>
+      <c r="E10" s="39" t="s">
+        <v>526</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>580</v>
+      </c>
+      <c r="G10" s="39" t="s">
+        <v>528</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>581</v>
+      </c>
+      <c r="I10" s="39" t="s">
+        <v>530</v>
+      </c>
+      <c r="J10" s="39" t="s">
+        <v>531</v>
+      </c>
+      <c r="K10" s="39" t="s">
+        <v>532</v>
+      </c>
+      <c r="L10" s="39" t="s">
+        <v>533</v>
+      </c>
+      <c r="M10" s="39" t="s">
+        <v>534</v>
+      </c>
+      <c r="N10" s="39" t="s">
+        <v>535</v>
+      </c>
+      <c r="O10" s="39" t="s">
+        <v>536</v>
+      </c>
+      <c r="P10" s="39" t="s">
+        <v>537</v>
+      </c>
+      <c r="Q10" s="39" t="s">
+        <v>538</v>
+      </c>
+      <c r="R10" s="39" t="s">
+        <v>539</v>
+      </c>
+      <c r="S10" s="39" t="s">
+        <v>540</v>
+      </c>
+      <c r="T10" s="39" t="s">
+        <v>541</v>
+      </c>
+      <c r="U10" s="39" t="s">
+        <v>542</v>
+      </c>
+      <c r="V10" s="39" t="s">
+        <v>543</v>
+      </c>
+      <c r="W10" s="39" t="s">
+        <v>544</v>
+      </c>
+      <c r="X10" s="39" t="s">
+        <v>545</v>
+      </c>
+      <c r="Y10" s="39" t="s">
+        <v>546</v>
+      </c>
+      <c r="Z10" s="39" t="s">
+        <v>547</v>
+      </c>
+      <c r="AA10" s="39" t="s">
+        <v>548</v>
+      </c>
+      <c r="AB10" s="39" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="39"/>
@@ -4852,13 +5048,13 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>
@@ -4888,13 +5084,13 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>613</v>
+        <v>554</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>466</v>
+        <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
@@ -4914,9 +5110,7 @@
       <c r="S13" s="39"/>
       <c r="T13" s="39"/>
       <c r="U13" s="39"/>
-      <c r="V13" s="55" t="b">
-        <v>1</v>
-      </c>
+      <c r="V13" s="39"/>
       <c r="W13" s="39"/>
       <c r="X13" s="39"/>
       <c r="Y13" s="39"/>
@@ -4926,82 +5120,170 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>555</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>466</v>
+        <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>467</v>
-      </c>
-      <c r="F14" t="s">
-        <v>561</v>
-      </c>
-      <c r="H14" t="s">
-        <v>561</v>
-      </c>
-      <c r="V14" t="s">
-        <v>468</v>
-      </c>
+        <v>559</v>
+      </c>
+      <c r="D14" s="39"/>
+      <c r="E14" s="39"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="39"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="39"/>
+      <c r="J14" s="39"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="39"/>
+      <c r="M14" s="39"/>
+      <c r="N14" s="39"/>
+      <c r="O14" s="39"/>
+      <c r="P14" s="39"/>
+      <c r="Q14" s="39"/>
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="39"/>
+      <c r="V14" s="39"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="39"/>
+      <c r="Y14" s="39"/>
+      <c r="Z14" s="39"/>
+      <c r="AA14" s="39"/>
+      <c r="AB14" s="39"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>621</v>
+        <v>612</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>618</v>
+        <v>465</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="J15" t="b">
+        <v>561</v>
+      </c>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="39"/>
+      <c r="G15" s="39"/>
+      <c r="H15" s="39"/>
+      <c r="I15" s="39"/>
+      <c r="J15" s="39"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="39"/>
+      <c r="M15" s="39"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="39"/>
+      <c r="P15" s="39"/>
+      <c r="Q15" s="39"/>
+      <c r="R15" s="39"/>
+      <c r="S15" s="39"/>
+      <c r="T15" s="39"/>
+      <c r="U15" s="39"/>
+      <c r="V15" s="55" t="b">
         <v>1</v>
       </c>
+      <c r="W15" s="39"/>
+      <c r="X15" s="39"/>
+      <c r="Y15" s="39"/>
+      <c r="Z15" s="39"/>
+      <c r="AA15" s="39"/>
+      <c r="AB15" s="39"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>625</v>
+        <v>185</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>618</v>
+        <v>465</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>626</v>
-      </c>
-      <c r="J16" t="b">
-        <v>1</v>
+        <v>466</v>
+      </c>
+      <c r="F16" t="s">
+        <v>560</v>
+      </c>
+      <c r="H16" t="s">
+        <v>560</v>
+      </c>
+      <c r="V16" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>624</v>
-      </c>
-      <c r="J17">
-        <v>200</v>
+        <v>621</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>624</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>625</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>622</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>617</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>623</v>
+      </c>
+      <c r="J19">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>626</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>627</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="D20" s="14" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>659</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>628</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>629</v>
+      <c r="C21" s="2" t="s">
+        <v>660</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>661</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:X12" xr:uid="{555E7DD2-3783-4E1D-82EE-0D15C5F56F09}"/>
+  <autoFilter ref="A1:X14" xr:uid="{555E7DD2-3783-4E1D-82EE-0D15C5F56F09}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -5060,37 +5342,37 @@
         <v>28</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C1" s="41" t="s">
+        <v>286</v>
+      </c>
+      <c r="D1" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="E1" s="41" t="s">
         <v>287</v>
       </c>
-      <c r="D1" s="41" t="s">
-        <v>286</v>
-      </c>
-      <c r="E1" s="41" t="s">
-        <v>288</v>
-      </c>
       <c r="F1" s="41" t="s">
+        <v>336</v>
+      </c>
+      <c r="G1" s="41" t="s">
         <v>337</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="H1" s="41" t="s">
         <v>338</v>
-      </c>
-      <c r="H1" s="41" t="s">
-        <v>339</v>
       </c>
       <c r="I1" s="41" t="s">
         <v>4</v>
       </c>
       <c r="J1" s="41" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="K1" s="45" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="L1" s="42" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="M1" s="41" t="s">
         <v>6</v>
@@ -5111,70 +5393,70 @@
         <v>1</v>
       </c>
       <c r="S1" s="41" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="T1" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="U1" s="41" t="s">
+        <v>308</v>
+      </c>
+      <c r="V1" s="41" t="s">
+        <v>309</v>
+      </c>
+      <c r="W1" s="41" t="s">
+        <v>310</v>
+      </c>
+      <c r="X1" s="41" t="s">
+        <v>311</v>
+      </c>
+      <c r="Y1" s="41" t="s">
+        <v>313</v>
+      </c>
+      <c r="Z1" s="41" t="s">
+        <v>312</v>
+      </c>
+      <c r="AA1" s="43" t="s">
+        <v>332</v>
+      </c>
+      <c r="AB1" s="43" t="s">
+        <v>317</v>
+      </c>
+      <c r="AC1" s="43" t="s">
+        <v>316</v>
+      </c>
+      <c r="AD1" s="41" t="s">
         <v>315</v>
       </c>
-      <c r="U1" s="41" t="s">
-        <v>309</v>
-      </c>
-      <c r="V1" s="41" t="s">
-        <v>310</v>
-      </c>
-      <c r="W1" s="41" t="s">
-        <v>311</v>
-      </c>
-      <c r="X1" s="41" t="s">
-        <v>312</v>
-      </c>
-      <c r="Y1" s="41" t="s">
-        <v>314</v>
-      </c>
-      <c r="Z1" s="41" t="s">
-        <v>313</v>
-      </c>
-      <c r="AA1" s="43" t="s">
+      <c r="AE1" s="41" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF1" s="41" t="s">
+        <v>318</v>
+      </c>
+      <c r="AG1" s="41" t="s">
+        <v>320</v>
+      </c>
+      <c r="AH1" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="AI1" s="45" t="s">
+        <v>329</v>
+      </c>
+      <c r="AJ1" s="45" t="s">
+        <v>331</v>
+      </c>
+      <c r="AK1" s="45" t="s">
         <v>333</v>
       </c>
-      <c r="AB1" s="43" t="s">
-        <v>318</v>
-      </c>
-      <c r="AC1" s="43" t="s">
-        <v>317</v>
-      </c>
-      <c r="AD1" s="41" t="s">
-        <v>316</v>
-      </c>
-      <c r="AE1" s="41" t="s">
-        <v>322</v>
-      </c>
-      <c r="AF1" s="41" t="s">
-        <v>319</v>
-      </c>
-      <c r="AG1" s="41" t="s">
-        <v>321</v>
-      </c>
-      <c r="AH1" s="41" t="s">
-        <v>320</v>
-      </c>
-      <c r="AI1" s="45" t="s">
+      <c r="AL1" s="45" t="s">
+        <v>334</v>
+      </c>
+      <c r="AM1" s="45" t="s">
+        <v>335</v>
+      </c>
+      <c r="AN1" s="45" t="s">
         <v>330</v>
-      </c>
-      <c r="AJ1" s="45" t="s">
-        <v>332</v>
-      </c>
-      <c r="AK1" s="45" t="s">
-        <v>334</v>
-      </c>
-      <c r="AL1" s="45" t="s">
-        <v>335</v>
-      </c>
-      <c r="AM1" s="45" t="s">
-        <v>336</v>
-      </c>
-      <c r="AN1" s="45" t="s">
-        <v>331</v>
       </c>
       <c r="AO1" s="41" t="s">
         <v>5</v>
@@ -5185,30 +5467,30 @@
     </row>
     <row r="2" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E2" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G2" s="39"/>
       <c r="H2" s="39"/>
       <c r="I2" s="39" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K2" s="46"/>
       <c r="L2" s="38"/>
@@ -5227,30 +5509,30 @@
     </row>
     <row r="3" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E3" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F3" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G3" s="39"/>
       <c r="H3" s="39"/>
       <c r="I3" s="39" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="J3" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K3" s="46"/>
       <c r="L3" s="38"/>
@@ -5269,30 +5551,30 @@
     </row>
     <row r="4" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E4" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F4" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G4" s="39"/>
       <c r="H4" s="39"/>
       <c r="I4" s="39" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K4" s="46"/>
       <c r="L4" s="38"/>
@@ -5311,30 +5593,30 @@
     </row>
     <row r="5" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B5" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E5" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F5" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G5" s="39"/>
       <c r="H5" s="39"/>
       <c r="I5" s="39" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="J5" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K5" s="46"/>
       <c r="L5" s="38"/>
@@ -5353,30 +5635,30 @@
     </row>
     <row r="6" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D6" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E6" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F6" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G6" s="39"/>
       <c r="H6" s="39"/>
       <c r="I6" s="39" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="J6" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K6" s="46"/>
       <c r="L6" s="38"/>
@@ -5395,30 +5677,30 @@
     </row>
     <row r="7" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B7" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D7" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E7" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F7" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G7" s="39"/>
       <c r="H7" s="39"/>
       <c r="I7" s="39" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K7" s="46"/>
       <c r="L7" s="38"/>
@@ -5437,30 +5719,30 @@
     </row>
     <row r="8" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B8" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D8" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E8" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F8" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G8" s="39"/>
       <c r="H8" s="39"/>
       <c r="I8" s="39" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="J8" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K8" s="46"/>
       <c r="L8" s="38"/>
@@ -5479,30 +5761,30 @@
     </row>
     <row r="9" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D9" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E9" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F9" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G9" s="39"/>
       <c r="H9" s="39"/>
       <c r="I9" s="39" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="J9" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K9" s="46"/>
       <c r="L9" s="38"/>
@@ -5521,30 +5803,30 @@
     </row>
     <row r="10" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C10" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D10" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E10" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G10" s="39"/>
       <c r="H10" s="39"/>
       <c r="I10" s="39" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="J10" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K10" s="46"/>
       <c r="L10" s="38"/>
@@ -5563,30 +5845,30 @@
     </row>
     <row r="11" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B11" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D11" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E11" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F11" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G11" s="39"/>
       <c r="H11" s="39"/>
       <c r="I11" s="39" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K11" s="46"/>
       <c r="L11" s="38"/>
@@ -5605,30 +5887,30 @@
     </row>
     <row r="12" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B12" t="s">
         <v>271</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D12" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E12" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F12" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G12" s="39"/>
       <c r="H12" s="39"/>
       <c r="I12" s="39" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="J12" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K12" s="46"/>
       <c r="L12" s="38"/>
@@ -5647,30 +5929,30 @@
     </row>
     <row r="13" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D13" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E13" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F13" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G13" s="39"/>
       <c r="H13" s="39"/>
       <c r="I13" s="39" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J13" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K13" s="46"/>
       <c r="L13" s="38"/>
@@ -5689,30 +5971,30 @@
     </row>
     <row r="14" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B14" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E14" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F14" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G14" s="39"/>
       <c r="H14" s="39"/>
       <c r="I14" s="39" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="J14" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K14" s="46"/>
       <c r="L14" s="38"/>
@@ -5731,30 +6013,30 @@
     </row>
     <row r="15" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D15" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E15" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F15" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G15" s="39"/>
       <c r="H15" s="39"/>
       <c r="I15" s="39" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="J15" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K15" s="46"/>
       <c r="L15" s="38"/>
@@ -5773,30 +6055,30 @@
     </row>
     <row r="16" spans="1:42" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B16" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E16" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F16" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G16" s="39"/>
       <c r="H16" s="39"/>
       <c r="I16" s="39" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="J16" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K16" s="46"/>
       <c r="L16" s="38"/>
@@ -5815,30 +6097,30 @@
     </row>
     <row r="17" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B17" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C17" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D17" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E17" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F17" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G17" s="39"/>
       <c r="H17" s="39"/>
       <c r="I17" s="39" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="J17" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K17" s="46"/>
       <c r="L17" s="38"/>
@@ -5857,30 +6139,30 @@
     </row>
     <row r="18" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D18" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E18" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F18" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G18" s="39"/>
       <c r="H18" s="39"/>
       <c r="I18" s="39" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="J18" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K18" s="46"/>
       <c r="L18" s="38"/>
@@ -5899,30 +6181,30 @@
     </row>
     <row r="19" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D19" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E19" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F19" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G19" s="39"/>
       <c r="H19" s="39"/>
       <c r="I19" s="39" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="J19" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K19" s="46"/>
       <c r="L19" s="38"/>
@@ -5941,30 +6223,30 @@
     </row>
     <row r="20" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B20" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D20" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E20" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F20" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G20" s="39"/>
       <c r="H20" s="39"/>
       <c r="I20" s="39" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="J20" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K20" s="46"/>
       <c r="L20" s="38"/>
@@ -5983,30 +6265,30 @@
     </row>
     <row r="21" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B21" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D21" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E21" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F21" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G21" s="39"/>
       <c r="H21" s="39"/>
       <c r="I21" s="39" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="J21" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K21" s="46"/>
       <c r="L21" s="38"/>
@@ -6025,30 +6307,30 @@
     </row>
     <row r="22" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B22" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C22" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D22" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E22" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F22" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G22" s="39"/>
       <c r="H22" s="39"/>
       <c r="I22" s="39" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="J22" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K22" s="46"/>
       <c r="L22" s="38"/>
@@ -6067,30 +6349,30 @@
     </row>
     <row r="23" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B23" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D23" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E23" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F23" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G23" s="39"/>
       <c r="H23" s="39"/>
       <c r="I23" s="39" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="J23" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K23" s="46"/>
       <c r="L23" s="38"/>
@@ -6109,30 +6391,30 @@
     </row>
     <row r="24" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B24" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C24" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D24" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E24" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F24" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G24" s="39"/>
       <c r="H24" s="39"/>
       <c r="I24" s="39" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="J24" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K24" s="46"/>
       <c r="L24" s="38"/>
@@ -6151,30 +6433,30 @@
     </row>
     <row r="25" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D25" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E25" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F25" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G25" s="39"/>
       <c r="H25" s="39"/>
       <c r="I25" s="39" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="J25" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K25" s="46"/>
       <c r="L25" s="38"/>
@@ -6193,30 +6475,30 @@
     </row>
     <row r="26" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B26" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D26" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E26" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F26" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G26" s="39"/>
       <c r="H26" s="39"/>
       <c r="I26" s="39" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="J26" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K26" s="46"/>
       <c r="L26" s="38"/>
@@ -6235,30 +6517,30 @@
     </row>
     <row r="27" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B27" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D27" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E27" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F27" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G27" s="39"/>
       <c r="H27" s="39"/>
       <c r="I27" s="39" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="J27" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K27" s="46"/>
       <c r="L27" s="38"/>
@@ -6277,30 +6559,30 @@
     </row>
     <row r="28" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B28" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D28" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E28" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F28" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G28" s="39"/>
       <c r="H28" s="39"/>
       <c r="I28" s="39" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="J28" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K28" s="46"/>
       <c r="L28" s="38"/>
@@ -6319,30 +6601,30 @@
     </row>
     <row r="29" spans="1:44" s="37" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B29" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D29" s="37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E29" s="39" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F29" s="39" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G29" s="39"/>
       <c r="H29" s="39"/>
       <c r="I29" s="39" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="J29" s="39" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K29" s="46"/>
       <c r="L29" s="38"/>
@@ -6361,31 +6643,31 @@
     </row>
     <row r="30" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>436</v>
+      </c>
+      <c r="C30" s="39" t="s">
+        <v>436</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>449</v>
+      </c>
+      <c r="E30" t="s">
+        <v>450</v>
+      </c>
+      <c r="F30" t="s">
+        <v>440</v>
+      </c>
+      <c r="I30" s="32" t="s">
+        <v>455</v>
+      </c>
+      <c r="J30" t="s">
         <v>437</v>
-      </c>
-      <c r="C30" s="39" t="s">
-        <v>437</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>450</v>
-      </c>
-      <c r="E30" t="s">
-        <v>451</v>
-      </c>
-      <c r="F30" t="s">
-        <v>441</v>
-      </c>
-      <c r="I30" s="32" t="s">
-        <v>456</v>
-      </c>
-      <c r="J30" t="s">
-        <v>438</v>
       </c>
       <c r="K30" s="6">
         <v>4326</v>
       </c>
       <c r="M30" s="48" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="N30" s="14">
         <v>20191101</v>
@@ -6397,16 +6679,16 @@
         <v>2015</v>
       </c>
       <c r="Q30" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="R30" t="s">
+        <v>438</v>
+      </c>
+      <c r="S30" s="36" t="s">
         <v>439</v>
       </c>
-      <c r="S30" s="36" t="s">
-        <v>440</v>
-      </c>
       <c r="T30" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="AA30"/>
       <c r="AB30"/>
@@ -6419,7 +6701,7 @@
       <c r="AJ30"/>
       <c r="AK30"/>
       <c r="AM30" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="AN30" s="6">
         <v>-200</v>
@@ -6431,25 +6713,25 @@
     </row>
     <row r="31" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="39" t="s">
+        <v>453</v>
+      </c>
+      <c r="C31" s="39" t="s">
+        <v>453</v>
+      </c>
+      <c r="D31" s="39" t="s">
         <v>454</v>
       </c>
-      <c r="C31" s="39" t="s">
-        <v>454</v>
-      </c>
-      <c r="D31" s="39" t="s">
-        <v>455</v>
-      </c>
       <c r="E31" s="39" t="s">
+        <v>451</v>
+      </c>
+      <c r="F31" s="39" t="s">
         <v>452</v>
       </c>
-      <c r="F31" s="39" t="s">
-        <v>453</v>
-      </c>
       <c r="I31" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="J31" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="K31" s="6">
         <v>4326</v>
@@ -6506,7 +6788,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B2" t="s">
         <v>205</v>
@@ -6521,7 +6803,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B3" t="s">
         <v>206</v>
@@ -6537,7 +6819,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B4" t="s">
         <v>207</v>
@@ -6553,7 +6835,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B5" t="s">
         <v>208</v>
@@ -6569,7 +6851,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B6" t="s">
         <v>209</v>
@@ -6647,13 +6929,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>457</v>
+      </c>
+      <c r="B11" t="s">
+        <v>423</v>
+      </c>
+      <c r="C11" t="s">
         <v>458</v>
-      </c>
-      <c r="B11" t="s">
-        <v>424</v>
-      </c>
-      <c r="C11" t="s">
-        <v>459</v>
       </c>
     </row>
   </sheetData>
@@ -6694,10 +6976,10 @@
         <v>174</v>
       </c>
       <c r="C1" s="59" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1" s="59" t="s">
         <v>460</v>
-      </c>
-      <c r="D1" s="59" t="s">
-        <v>461</v>
       </c>
       <c r="E1" s="59" t="s">
         <v>176</v>
@@ -6709,7 +6991,7 @@
         <v>179</v>
       </c>
       <c r="H1" s="59" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I1" s="60" t="s">
         <v>32</v>
@@ -6724,10 +7006,10 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B2" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B2" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>205</v>
@@ -6755,10 +7037,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B3" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>205</v>
@@ -6784,10 +7066,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B4" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B4" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>205</v>
@@ -6813,10 +7095,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B5" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B5" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>205</v>
@@ -6844,10 +7126,10 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B6" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B6" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>205</v>
@@ -6873,10 +7155,10 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B7" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B7" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>206</v>
@@ -6906,10 +7188,10 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B8" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B8" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>206</v>
@@ -6939,10 +7221,10 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B9" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B9" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>206</v>
@@ -6951,10 +7233,10 @@
         <v>225</v>
       </c>
       <c r="E9" s="62" t="s">
+        <v>463</v>
+      </c>
+      <c r="F9" s="62" t="s">
         <v>464</v>
-      </c>
-      <c r="F9" s="62" t="s">
-        <v>465</v>
       </c>
       <c r="G9" s="63"/>
       <c r="H9" s="63"/>
@@ -6964,10 +7246,10 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B10" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B10" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>207</v>
@@ -6997,10 +7279,10 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B11" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B11" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>207</v>
@@ -7030,10 +7312,10 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B12" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B12" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>207</v>
@@ -7061,10 +7343,10 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B13" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B13" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>208</v>
@@ -7094,10 +7376,10 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B14" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B14" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>208</v>
@@ -7123,10 +7405,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B15" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B15" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>208</v>
@@ -7152,10 +7434,10 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B16" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B16" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>208</v>
@@ -7181,10 +7463,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B17" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B17" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>209</v>
@@ -7214,10 +7496,10 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B18" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B18" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>209</v>
@@ -7247,10 +7529,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B19" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B19" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>259</v>
@@ -7280,10 +7562,10 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B20" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B20" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>259</v>
@@ -7311,10 +7593,10 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B21" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B21" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>259</v>
@@ -7342,10 +7624,10 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B22" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B22" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>259</v>
@@ -7373,10 +7655,10 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B23" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B23" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>259</v>
@@ -7402,10 +7684,10 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="B24" s="62" t="s">
         <v>462</v>
-      </c>
-      <c r="B24" s="62" t="s">
-        <v>463</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>259</v>
@@ -7615,349 +7897,349 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>426</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="C32" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>426</v>
-      </c>
       <c r="F32" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="C33" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D33" s="3" t="s">
         <v>424</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>425</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>215</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B34" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="C34" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D34" s="3" t="s">
         <v>424</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>425</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>215</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="C35" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="E35" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>424</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>425</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>426</v>
-      </c>
       <c r="F36" s="3" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="J36" s="33"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B37" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="C37" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D37" s="3" t="s">
         <v>424</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>425</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J37" s="33"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="C38" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D38" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="E38" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J38" s="33"/>
       <c r="K38" s="34"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B39" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="C39" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="D39" s="3" t="s">
         <v>424</v>
       </c>
-      <c r="D39" s="3" t="s">
-        <v>425</v>
-      </c>
       <c r="E39" s="3" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J39" s="33"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>585</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>584</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>586</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="G40" s="63">
         <v>924972</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J40" s="33"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="G41" s="63">
         <v>356890</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="J41" s="33"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="G42" s="63">
         <v>6309</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J42" s="33"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>591</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>592</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="G43" s="63">
         <v>326229</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>594</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>595</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="G44" s="63">
         <v>151404</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>597</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>598</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="G45" s="63">
         <v>156117</v>
       </c>
       <c r="I45" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>603</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>604</v>
       </c>
     </row>
   </sheetData>
@@ -7970,8 +8252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD6A12AB-4082-428A-9AD8-30AFCF82C953}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7986,74 +8268,74 @@
   <sheetData>
     <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>493</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>507</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>506</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>500</v>
+      </c>
+      <c r="F1" s="10" t="s">
         <v>494</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>496</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>508</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>507</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>501</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>495</v>
-      </c>
       <c r="G1" s="10" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="H1" s="58" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="G2" s="57" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H2" s="57" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C3" s="54" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="G3" s="57" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="H3" s="57" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -8061,25 +8343,25 @@
         <v>127</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G4" s="57" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H4" s="57" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -8087,155 +8369,155 @@
         <v>129</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C5" s="54" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="G5" s="57" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H5" s="57" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="G6" s="57" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="H6" s="57" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G7" s="57" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="H7" s="57" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>509</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>508</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>571</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="C8" s="54" t="s">
-        <v>510</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>509</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>572</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="G8" s="57" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="H8" s="57" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C9" s="54" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="G9" s="57" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H9" s="57" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C10" s="54" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="G10" s="57" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="H10" s="57" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -8243,19 +8525,19 @@
         <v>147</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="G11" s="57" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="H11" s="57" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -8263,25 +8545,25 @@
         <v>149</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C12" s="54" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="G12" s="57" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="H12" s="57" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="120" x14ac:dyDescent="0.25">
@@ -8289,23 +8571,23 @@
         <v>151</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C13" s="54"/>
       <c r="D13" s="3" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G13" s="57" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="H13" s="57" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="409.5" x14ac:dyDescent="0.25">
@@ -8313,25 +8595,25 @@
         <v>155</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C14" s="3" t="s">
+        <v>517</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>518</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>519</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G14" s="57" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="H14" s="57" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -8339,22 +8621,22 @@
         <v>157</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C15" s="54" t="s">
+        <v>566</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>518</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>505</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>567</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>506</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>568</v>
-      </c>
       <c r="G15" s="57" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H15" s="57" t="s">
         <v>214</v>

</xml_diff>

<commit_message>
updated docker image so main build is in one RUN statement (the seperate runs for small tasks launching python are still present as in original); quickly test built and appears to work as intended, so that looks good.
</commit_message>
<xml_diff>
--- a/process/pre_process/_project_configuration.xlsx
+++ b/process/pre_process/_project_configuration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\global-indicators\process\pre_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0ACAD3E-4D96-4C1F-B50C-D9B5B8A312D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCFD967-2CC2-4D3A-9B4D-C7CAE8131E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4160,7 +4160,7 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Draft re-parameterisation code (1000km instead of 1600m walkable neightbourhoods, and exclude urban sample points where located in intersection with a hex grid cell with population estimate below a minimum threshold value of 5).  Also tidied up output locations to ensure both the address level output and city level outputs are generated in the output folder, and the node csv is no longer 'tempCSV' but properly named as a parameter, and is likewise considered an output, not an input
</commit_message>
<xml_diff>
--- a/process/pre_process/_project_configuration.xlsx
+++ b/process/pre_process/_project_configuration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\global-indicators\process\pre_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABCFD967-2CC2-4D3A-9B4D-C7CAE8131E61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC76404E-D1D6-4F00-AE56-4BC6833EAEC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="16" r:id="rId1"/>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="662">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="664">
   <si>
     <t>notes</t>
   </si>
@@ -2130,6 +2130,12 @@
   </si>
   <si>
     <t>Dr Garba Sambo (University of Maiduguri) and Assoc. Prof. Adewale Oyeyemi (University of Maiduguri)</t>
+  </si>
+  <si>
+    <t>pop_min_threshold</t>
+  </si>
+  <si>
+    <t>urban sample points intersecting hex grid cells with estimated population less than this will be excluded from analysis</t>
   </si>
 </sst>
 </file>
@@ -3601,10 +3607,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF89BF1A-C929-463D-A334-3406512FE43F}">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4136,15 +4142,29 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>662</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="D38" s="14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>446</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B39" s="2" t="s">
         <v>447</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="C39" s="2" t="s">
         <v>608</v>
       </c>
-      <c r="D38" s="14" t="s">
+      <c r="D39" s="14" t="s">
         <v>453</v>
       </c>
     </row>
@@ -4159,7 +4179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737B355D-4426-4406-A37B-14B20C191AA3}">
   <dimension ref="A1:AB21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added in new urban covariates dataset, with initial draft of code for urban region population, intersections, and optional linkage covariates (ie. GHS air pollution statistics); also inconsequential modification of open space script, with removal of some redundant end of line spaces (no practical impact, beyond neatness)
</commit_message>
<xml_diff>
--- a/process/pre_process/_project_configuration.xlsx
+++ b/process/pre_process/_project_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\global-indicators\process\pre_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC76404E-D1D6-4F00-AE56-4BC6833EAEC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D03631-0FC6-4222-A783-4C4BBFC19DB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="16" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="destinations" sheetId="26" r:id="rId5"/>
     <sheet name="osm_dest_definitions" sheetId="25" r:id="rId6"/>
     <sheet name="osm_open_space" sheetId="29" r:id="rId7"/>
+    <sheet name="covariate data" sheetId="30" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">datasets!$A$1:$AP$29</definedName>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="705">
   <si>
     <t>notes</t>
   </si>
@@ -1784,9 +1785,6 @@
     <t>./data/boundaries.gpkg:Perth</t>
   </si>
   <si>
-    <t>Region boundary data</t>
-  </si>
-  <si>
     <t>area_data_source</t>
   </si>
   <si>
@@ -2136,6 +2134,132 @@
   </si>
   <si>
     <t>urban sample points intersecting hex grid cells with estimated population less than this will be excluded from analysis</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Mexico City'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Phoenix'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='SÃ£o Paulo'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Hong Kong'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Chennai'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Bangkok'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Hanoi'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Graz'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Ghent'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Bern'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Olomouc'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Cologne'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Odense'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Barcelona'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Valencia'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Belfast'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Lisbon'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Adelaide'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Melbourne'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Sydney'</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='Auckland'</t>
+  </si>
+  <si>
+    <t>Region boundary data (path relative to project directory, or GHS:variable='value')</t>
+  </si>
+  <si>
+    <t>covariates</t>
+  </si>
+  <si>
+    <t>comma seperated list of additional air pollution covariate variables to be linked for study regions</t>
+  </si>
+  <si>
+    <t>E_EC2E_T15,E_EC2O_T15,E_EPM2_T15,E_CPM2_T14</t>
+  </si>
+  <si>
+    <t>Air pollution</t>
+  </si>
+  <si>
+    <t>Additional data linkage of study region covariates is defined in project and region settings.  These variables are defined here.</t>
+  </si>
+  <si>
+    <t>Total emission of CO 2 from the transport sector, using non-short-cycle-organic fuels in 2015</t>
+  </si>
+  <si>
+    <t>Total emission of CO 2 from the energy sector, using short-cycle-organic fuels in 2015</t>
+  </si>
+  <si>
+    <t>Total emission of PM 2.5 from the transport sector in 2015</t>
+  </si>
+  <si>
+    <t>E_EC2E_T15</t>
+  </si>
+  <si>
+    <t>E_EC2O_T15</t>
+  </si>
+  <si>
+    <t>E_EPM2_T15</t>
+  </si>
+  <si>
+    <t>E_CPM2_T14</t>
+  </si>
+  <si>
+    <t>Total concertation of PM 2.5 for reference epoch 2014</t>
+  </si>
+  <si>
+    <t>The GHS UCDB (1.2) is to be used where available (all cities, except Vic) for linkage of Urban Centre scale estimates of the following air pollution measures</t>
+  </si>
+  <si>
+    <t>For Vic, it may be possible to locate equivalent estimate, so the capability of linkage of a complimentary dataset of air pollution covariates using these variable names (e.g. a custom prepared CSV based on estimates from a separate data source) may be implemented pending capacity to code and locate such estimates</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>covariate_data</t>
+  </si>
+  <si>
+    <t>GHS or other linkage of covariate data (GHS:variable='value', or path:variable='value' for a dataset with equivalently named fields defined in project parameters for air_pollution_covariates)</t>
+  </si>
+  <si>
+    <t>linkage_covariate_list</t>
   </si>
 </sst>
 </file>
@@ -3607,10 +3731,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF89BF1A-C929-463D-A334-3406512FE43F}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3646,7 +3770,7 @@
         <v>35</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3702,7 +3826,7 @@
         <v>296</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3769,7 +3893,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D11" s="14">
         <v>2020</v>
@@ -3856,7 +3980,7 @@
         <v>281</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -3881,7 +4005,7 @@
         <v>294</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D19" s="14" t="str">
         <f>"False"</f>
@@ -4120,7 +4244,7 @@
         <v>436</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>436</v>
@@ -4142,13 +4266,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>436</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="D38" s="14">
         <v>5</v>
@@ -4162,10 +4286,24 @@
         <v>447</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D39" s="14" t="s">
         <v>453</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>704</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>686</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>687</v>
       </c>
     </row>
   </sheetData>
@@ -4177,10 +4315,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737B355D-4426-4406-A37B-14B20C191AA3}">
-  <dimension ref="A1:AB21"/>
+  <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4546,7 +4684,7 @@
         <v>277</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>413</v>
@@ -4626,174 +4764,174 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>277</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E6" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F6" t="s">
+        <v>637</v>
+      </c>
+      <c r="G6" t="s">
+        <v>637</v>
+      </c>
+      <c r="H6" t="s">
+        <v>637</v>
+      </c>
+      <c r="I6" t="s">
         <v>638</v>
       </c>
-      <c r="G6" t="s">
-        <v>638</v>
-      </c>
-      <c r="H6" t="s">
-        <v>638</v>
-      </c>
-      <c r="I6" t="s">
-        <v>639</v>
-      </c>
       <c r="J6" t="s">
+        <v>656</v>
+      </c>
+      <c r="K6" t="s">
+        <v>641</v>
+      </c>
+      <c r="L6" t="s">
+        <v>642</v>
+      </c>
+      <c r="M6" t="s">
+        <v>643</v>
+      </c>
+      <c r="N6" t="s">
+        <v>644</v>
+      </c>
+      <c r="O6" t="s">
+        <v>646</v>
+      </c>
+      <c r="P6" t="s">
+        <v>647</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>648</v>
+      </c>
+      <c r="R6" t="s">
+        <v>649</v>
+      </c>
+      <c r="S6" t="s">
+        <v>650</v>
+      </c>
+      <c r="T6" t="s">
+        <v>651</v>
+      </c>
+      <c r="U6" t="s">
+        <v>651</v>
+      </c>
+      <c r="V6" t="s">
+        <v>651</v>
+      </c>
+      <c r="W6" t="s">
         <v>657</v>
       </c>
-      <c r="K6" t="s">
-        <v>642</v>
-      </c>
-      <c r="L6" t="s">
-        <v>643</v>
-      </c>
-      <c r="M6" t="s">
-        <v>644</v>
-      </c>
-      <c r="N6" t="s">
-        <v>645</v>
-      </c>
-      <c r="O6" t="s">
-        <v>647</v>
-      </c>
-      <c r="P6" t="s">
-        <v>648</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>649</v>
-      </c>
-      <c r="R6" t="s">
-        <v>650</v>
-      </c>
-      <c r="S6" t="s">
-        <v>651</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="X6" t="s">
         <v>652</v>
       </c>
-      <c r="U6" t="s">
-        <v>652</v>
-      </c>
-      <c r="V6" t="s">
-        <v>652</v>
-      </c>
-      <c r="W6" t="s">
-        <v>658</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="Y6" s="14" t="s">
         <v>653</v>
       </c>
-      <c r="Y6" s="14" t="s">
-        <v>654</v>
-      </c>
       <c r="Z6" s="14" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="AA6" s="14" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="AB6" s="14" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>277</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="G7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="H7" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I7" t="s">
+        <v>639</v>
+      </c>
+      <c r="J7" t="s">
         <v>640</v>
       </c>
-      <c r="J7" t="s">
-        <v>641</v>
-      </c>
       <c r="K7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="L7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="M7" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="N7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="O7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="P7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="Q7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="R7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="S7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="T7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="U7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="V7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="W7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="X7" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="Y7" s="14" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="Z7" s="14" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="AA7" s="14" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="AB7" s="14" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="8" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -4952,22 +5090,22 @@
         <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>551</v>
+        <v>684</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="E10" s="39" t="s">
         <v>526</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="G10" s="39" t="s">
         <v>528</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I10" s="39" t="s">
         <v>530</v>
@@ -5032,13 +5170,13 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D11" s="39"/>
       <c r="E11" s="39"/>
@@ -5068,13 +5206,13 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D12" s="39"/>
       <c r="E12" s="39"/>
@@ -5104,13 +5242,13 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D13" s="39"/>
       <c r="E13" s="39"/>
@@ -5140,13 +5278,13 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>59</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D14" s="39"/>
       <c r="E14" s="39"/>
@@ -5176,13 +5314,13 @@
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>465</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="39"/>
@@ -5223,83 +5361,166 @@
         <v>466</v>
       </c>
       <c r="F16" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="H16" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="V16" t="s">
         <v>467</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>619</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>620</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>621</v>
       </c>
       <c r="J17" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>623</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>624</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>625</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>621</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>616</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>622</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>617</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>623</v>
       </c>
       <c r="J19">
         <v>200</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>626</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>627</v>
       </c>
-      <c r="D20" s="14" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>660</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>661</v>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>702</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="D22" t="s">
+        <v>581</v>
+      </c>
+      <c r="E22" t="s">
+        <v>663</v>
+      </c>
+      <c r="F22" t="s">
+        <v>579</v>
+      </c>
+      <c r="G22" t="s">
+        <v>664</v>
+      </c>
+      <c r="H22" t="s">
+        <v>580</v>
+      </c>
+      <c r="I22" t="s">
+        <v>665</v>
+      </c>
+      <c r="J22" t="s">
+        <v>666</v>
+      </c>
+      <c r="K22" t="s">
+        <v>667</v>
+      </c>
+      <c r="L22" t="s">
+        <v>668</v>
+      </c>
+      <c r="M22" t="s">
+        <v>669</v>
+      </c>
+      <c r="N22" t="s">
+        <v>670</v>
+      </c>
+      <c r="O22" t="s">
+        <v>671</v>
+      </c>
+      <c r="P22" t="s">
+        <v>672</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>673</v>
+      </c>
+      <c r="R22" t="s">
+        <v>674</v>
+      </c>
+      <c r="S22" t="s">
+        <v>675</v>
+      </c>
+      <c r="T22" t="s">
+        <v>676</v>
+      </c>
+      <c r="U22" t="s">
+        <v>677</v>
+      </c>
+      <c r="W22" t="s">
+        <v>678</v>
+      </c>
+      <c r="X22" t="s">
+        <v>679</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>680</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>681</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>682</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>683</v>
       </c>
     </row>
   </sheetData>
@@ -6748,7 +6969,7 @@
         <v>452</v>
       </c>
       <c r="I31" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="J31" t="s">
         <v>291</v>
@@ -8102,164 +8323,164 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
+        <v>583</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>582</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>584</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>583</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>585</v>
-      </c>
       <c r="D40" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="G40" s="63">
         <v>924972</v>
       </c>
       <c r="I40" s="9" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="J40" s="33"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E41" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="G41" s="63">
         <v>356890</v>
       </c>
       <c r="I41" s="9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="J41" s="33"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="G42" s="63">
         <v>6309</v>
       </c>
       <c r="I42" s="9" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="J42" s="33"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="C43" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>590</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>591</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="G43" s="63">
         <v>326229</v>
       </c>
       <c r="I43" s="9" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C44" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>593</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>594</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="G44" s="63">
         <v>151404</v>
       </c>
       <c r="I44" s="9" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="C45" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>596</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>597</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>213</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="G45" s="63">
         <v>156117</v>
       </c>
       <c r="I45" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="K45" s="3" t="s">
         <v>602</v>
-      </c>
-      <c r="K45" s="3" t="s">
-        <v>603</v>
       </c>
     </row>
   </sheetData>
@@ -8306,10 +8527,10 @@
         <v>494</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="H1" s="58" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -8320,13 +8541,13 @@
         <v>496</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G2" s="57" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="H2" s="57" t="s">
         <v>480</v>
@@ -8346,13 +8567,13 @@
         <v>511</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="G3" s="57" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="H3" s="57" t="s">
         <v>510</v>
@@ -8372,13 +8593,13 @@
         <v>508</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="G4" s="57" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="H4" s="57" t="s">
         <v>481</v>
@@ -8401,10 +8622,10 @@
         <v>501</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="G5" s="57" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="H5" s="57" t="s">
         <v>482</v>
@@ -8464,7 +8685,7 @@
     </row>
     <row r="8" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>496</v>
@@ -8476,13 +8697,13 @@
         <v>508</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="G8" s="57" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="H8" s="57" t="s">
         <v>484</v>
@@ -8502,7 +8723,7 @@
         <v>508</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>487</v>
@@ -8516,7 +8737,7 @@
     </row>
     <row r="10" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>496</v>
@@ -8528,7 +8749,7 @@
         <v>508</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>486</v>
@@ -8624,13 +8845,13 @@
         <v>518</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="G14" s="57" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="H14" s="57" t="s">
         <v>514</v>
@@ -8644,7 +8865,7 @@
         <v>496</v>
       </c>
       <c r="C15" s="54" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>518</v>
@@ -8653,10 +8874,10 @@
         <v>505</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G15" s="57" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="H15" s="57" t="s">
         <v>214</v>
@@ -8665,4 +8886,83 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29433C24-917B-40F5-B064-66F51A7E075E}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>700</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>693</v>
+      </c>
+      <c r="B7" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>694</v>
+      </c>
+      <c r="B8" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>695</v>
+      </c>
+      <c r="B9" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>696</v>
+      </c>
+      <c r="B10" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>699</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
corrected unicode name of Sao Paulo for linkage with GHS urban layer covariates (ie. São Paulo)
</commit_message>
<xml_diff>
--- a/process/pre_process/_project_configuration.xlsx
+++ b/process/pre_process/_project_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\global-indicators\process\pre_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9D03631-0FC6-4222-A783-4C4BBFC19DB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F63A6F5-E5A0-4BE4-989F-4EF0283F503B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="16" r:id="rId1"/>
@@ -2142,9 +2142,6 @@
     <t>GHS:UC_NM_MN='Phoenix'</t>
   </si>
   <si>
-    <t>GHS:UC_NM_MN='SÃ£o Paulo'</t>
-  </si>
-  <si>
     <t>GHS:UC_NM_MN='Hong Kong'</t>
   </si>
   <si>
@@ -2260,6 +2257,9 @@
   </si>
   <si>
     <t>linkage_covariate_list</t>
+  </si>
+  <si>
+    <t>GHS:UC_NM_MN='São Paulo'</t>
   </si>
 </sst>
 </file>
@@ -3733,7 +3733,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF89BF1A-C929-463D-A334-3406512FE43F}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
@@ -4294,16 +4294,16 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>685</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="14" t="s">
         <v>686</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>687</v>
       </c>
     </row>
   </sheetData>
@@ -4317,8 +4317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737B355D-4426-4406-A37B-14B20C191AA3}">
   <dimension ref="A1:AB22"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5090,7 +5090,7 @@
         <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>581</v>
@@ -5442,13 +5442,13 @@
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>701</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>684</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>702</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>685</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>703</v>
       </c>
       <c r="D22" t="s">
         <v>581</v>
@@ -5466,61 +5466,61 @@
         <v>580</v>
       </c>
       <c r="I22" t="s">
+        <v>704</v>
+      </c>
+      <c r="J22" t="s">
         <v>665</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>666</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>667</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>668</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>669</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>670</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>671</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>672</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" t="s">
         <v>673</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>674</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>675</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>676</v>
       </c>
-      <c r="U22" t="s">
+      <c r="W22" t="s">
         <v>677</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
         <v>678</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>679</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>680</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AA22" t="s">
         <v>681</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AB22" t="s">
         <v>682</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>683</v>
       </c>
     </row>
   </sheetData>
@@ -8903,62 +8903,62 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>700</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B7" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B8" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B9" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>695</v>
+      </c>
+      <c r="B10" t="s">
         <v>696</v>
-      </c>
-      <c r="B10" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated notes on ambient pollution covariates (added in units and notes on interpretation of units in plain language, in addition to descriptions)
</commit_message>
<xml_diff>
--- a/process/pre_process/_project_configuration.xlsx
+++ b/process/pre_process/_project_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\global-indicators\process\pre_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F63A6F5-E5A0-4BE4-989F-4EF0283F503B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F6D03A-5A9F-431F-B372-2DE604F9EFC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="16" r:id="rId1"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1394" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1405" uniqueCount="712">
   <si>
     <t>notes</t>
   </si>
@@ -2260,6 +2260,27 @@
   </si>
   <si>
     <t>GHS:UC_NM_MN='São Paulo'</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>μg m⁻³</t>
+  </si>
+  <si>
+    <t>t a⁻¹</t>
+  </si>
+  <si>
+    <t>tonnes per annum</t>
+  </si>
+  <si>
+    <t>Unit description</t>
+  </si>
+  <si>
+    <t>micrograms per cubic meter</t>
+  </si>
+  <si>
+    <t>Note that notation raised to a negative power is another way of saying "per"; e.g. μg m⁻³ is equivalent to μg/m³ , just as both 10⁻³  and 1/(10³) are equal to 0.001 or 1/1000</t>
   </si>
 </sst>
 </file>
@@ -2438,7 +2459,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2619,6 +2640,7 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -4317,7 +4339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737B355D-4426-4406-A37B-14B20C191AA3}">
   <dimension ref="A1:AB22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
@@ -8890,76 +8912,118 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29433C24-917B-40F5-B064-66F51A7E075E}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>687</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>697</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>699</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>709</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>700</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>692</v>
       </c>
       <c r="B7" t="s">
+        <v>707</v>
+      </c>
+      <c r="C7" t="s">
+        <v>708</v>
+      </c>
+      <c r="D7" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>693</v>
       </c>
       <c r="B8" t="s">
+        <v>707</v>
+      </c>
+      <c r="C8" t="s">
+        <v>708</v>
+      </c>
+      <c r="D8" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>694</v>
       </c>
       <c r="B9" t="s">
+        <v>707</v>
+      </c>
+      <c r="C9" t="s">
+        <v>708</v>
+      </c>
+      <c r="D9" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>695</v>
       </c>
       <c r="B10" t="s">
+        <v>706</v>
+      </c>
+      <c r="C10" t="s">
+        <v>710</v>
+      </c>
+      <c r="D10" t="s">
         <v>696</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>698</v>
       </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="68" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="68"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
simplified the network creation script (removed an unused option to rebuild graph - this is False in the code, so optional loop for not false is not required), and refined the export gpkg code (if gpkg exists delete, but then add tables one at a time --- I think this seems the fastest way while providing feedback on progress of saving to the user)
</commit_message>
<xml_diff>
--- a/process/pre_process/_project_configuration.xlsx
+++ b/process/pre_process/_project_configuration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\global-indicators\process\pre_process\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAFF26D-012C-49D6-A1BD-D8B59823B3C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99C90106-3B9C-4C30-9128-727DB00C73FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="16" r:id="rId1"/>
@@ -2016,9 +2016,6 @@
     <t>network_polygon_iteration</t>
   </si>
   <si>
-    <t>Iterate over polygons for network retrieval, and then combin</t>
-  </si>
-  <si>
     <t>custom_destinations</t>
   </si>
   <si>
@@ -2278,6 +2275,9 @@
   </si>
   <si>
     <t>Note that notation raised to a negative power is another way of saying "per"; e.g. μg m⁻³ is equivalent to μg/m³ , just as both 10⁻³  and 1/(10³) are equal to 0.001 or 1/1000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iterate over polygons for network retrieval, and then combine </t>
   </si>
 </sst>
 </file>
@@ -2972,7 +2972,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D88"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -3750,8 +3750,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF89BF1A-C929-463D-A334-3406512FE43F}">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4283,13 +4283,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>435</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D38" s="14">
         <v>5</v>
@@ -4311,16 +4311,16 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>683</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="14" t="s">
         <v>684</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -4334,8 +4334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737B355D-4426-4406-A37B-14B20C191AA3}">
   <dimension ref="A1:AB22"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4701,7 +4701,7 @@
         <v>276</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="D5" s="14" t="s">
         <v>412</v>
@@ -4781,174 +4781,174 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>276</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E6" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F6" t="s">
+        <v>635</v>
+      </c>
+      <c r="G6" t="s">
+        <v>635</v>
+      </c>
+      <c r="H6" t="s">
+        <v>635</v>
+      </c>
+      <c r="I6" t="s">
         <v>636</v>
       </c>
-      <c r="G6" t="s">
-        <v>636</v>
-      </c>
-      <c r="H6" t="s">
-        <v>636</v>
-      </c>
-      <c r="I6" t="s">
-        <v>637</v>
-      </c>
       <c r="J6" t="s">
+        <v>654</v>
+      </c>
+      <c r="K6" t="s">
+        <v>639</v>
+      </c>
+      <c r="L6" t="s">
+        <v>640</v>
+      </c>
+      <c r="M6" t="s">
+        <v>641</v>
+      </c>
+      <c r="N6" t="s">
+        <v>642</v>
+      </c>
+      <c r="O6" t="s">
+        <v>644</v>
+      </c>
+      <c r="P6" t="s">
+        <v>645</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>646</v>
+      </c>
+      <c r="R6" t="s">
+        <v>647</v>
+      </c>
+      <c r="S6" t="s">
+        <v>648</v>
+      </c>
+      <c r="T6" t="s">
+        <v>649</v>
+      </c>
+      <c r="U6" t="s">
+        <v>649</v>
+      </c>
+      <c r="V6" t="s">
+        <v>649</v>
+      </c>
+      <c r="W6" t="s">
         <v>655</v>
       </c>
-      <c r="K6" t="s">
-        <v>640</v>
-      </c>
-      <c r="L6" t="s">
-        <v>641</v>
-      </c>
-      <c r="M6" t="s">
-        <v>642</v>
-      </c>
-      <c r="N6" t="s">
-        <v>643</v>
-      </c>
-      <c r="O6" t="s">
-        <v>645</v>
-      </c>
-      <c r="P6" t="s">
-        <v>646</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>647</v>
-      </c>
-      <c r="R6" t="s">
-        <v>648</v>
-      </c>
-      <c r="S6" t="s">
-        <v>649</v>
-      </c>
-      <c r="T6" t="s">
+      <c r="X6" t="s">
         <v>650</v>
       </c>
-      <c r="U6" t="s">
-        <v>650</v>
-      </c>
-      <c r="V6" t="s">
-        <v>650</v>
-      </c>
-      <c r="W6" t="s">
-        <v>656</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="Y6" s="14" t="s">
         <v>651</v>
       </c>
-      <c r="Y6" s="14" t="s">
-        <v>652</v>
-      </c>
       <c r="Z6" s="14" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AA6" s="14" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="AB6" s="14" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>276</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="E7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="G7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="H7" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I7" t="s">
+        <v>637</v>
+      </c>
+      <c r="J7" t="s">
         <v>638</v>
       </c>
-      <c r="J7" t="s">
-        <v>639</v>
-      </c>
       <c r="K7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="L7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="M7" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="N7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="O7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="P7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="Q7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="R7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="S7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="T7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="U7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="V7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="W7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="X7" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="Y7" s="14" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="Z7" s="14" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="AA7" s="14" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="AB7" s="14" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="8" spans="1:28" s="14" customFormat="1" x14ac:dyDescent="0.25">
@@ -5107,7 +5107,7 @@
         <v>59</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D10" s="14" t="s">
         <v>580</v>
@@ -5409,7 +5409,7 @@
         <v>615</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>623</v>
+        <v>710</v>
       </c>
       <c r="J18" t="b">
         <v>1</v>
@@ -5431,113 +5431,113 @@
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>624</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>625</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>82</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>657</v>
+      </c>
+      <c r="D21" s="14" t="s">
         <v>658</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>659</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>699</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>682</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>700</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>683</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>701</v>
       </c>
       <c r="D22" t="s">
         <v>580</v>
       </c>
       <c r="E22" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="F22" t="s">
         <v>578</v>
       </c>
       <c r="G22" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="H22" t="s">
         <v>579</v>
       </c>
       <c r="I22" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="J22" t="s">
+        <v>663</v>
+      </c>
+      <c r="K22" t="s">
         <v>664</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>665</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>666</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>667</v>
       </c>
-      <c r="N22" t="s">
+      <c r="O22" t="s">
         <v>668</v>
       </c>
-      <c r="O22" t="s">
+      <c r="P22" t="s">
         <v>669</v>
       </c>
-      <c r="P22" t="s">
+      <c r="Q22" t="s">
         <v>670</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" t="s">
         <v>671</v>
       </c>
-      <c r="R22" t="s">
+      <c r="S22" t="s">
         <v>672</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>673</v>
       </c>
-      <c r="T22" t="s">
+      <c r="U22" t="s">
         <v>674</v>
       </c>
-      <c r="U22" t="s">
+      <c r="W22" t="s">
         <v>675</v>
       </c>
-      <c r="W22" t="s">
+      <c r="X22" t="s">
         <v>676</v>
       </c>
-      <c r="X22" t="s">
+      <c r="Y22" t="s">
         <v>677</v>
       </c>
-      <c r="Y22" t="s">
+      <c r="Z22" t="s">
         <v>678</v>
       </c>
-      <c r="Z22" t="s">
+      <c r="AA22" t="s">
         <v>679</v>
       </c>
-      <c r="AA22" t="s">
+      <c r="AB22" t="s">
         <v>680</v>
-      </c>
-      <c r="AB22" t="s">
-        <v>681</v>
       </c>
     </row>
   </sheetData>
@@ -8922,99 +8922,99 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>697</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>703</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>707</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>698</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>704</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>708</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>699</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B7" t="s">
+        <v>705</v>
+      </c>
+      <c r="C7" t="s">
         <v>706</v>
       </c>
-      <c r="C7" t="s">
-        <v>707</v>
-      </c>
       <c r="D7" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="B8" t="s">
+        <v>705</v>
+      </c>
+      <c r="C8" t="s">
         <v>706</v>
       </c>
-      <c r="C8" t="s">
-        <v>707</v>
-      </c>
       <c r="D8" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B9" t="s">
+        <v>705</v>
+      </c>
+      <c r="C9" t="s">
         <v>706</v>
       </c>
-      <c r="C9" t="s">
-        <v>707</v>
-      </c>
       <c r="D9" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>693</v>
+      </c>
+      <c r="B10" t="s">
+        <v>704</v>
+      </c>
+      <c r="C10" t="s">
+        <v>708</v>
+      </c>
+      <c r="D10" t="s">
         <v>694</v>
-      </c>
-      <c r="B10" t="s">
-        <v>705</v>
-      </c>
-      <c r="C10" t="s">
-        <v>709</v>
-      </c>
-      <c r="D10" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="68" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>